<commit_message>
skipp comment and new example
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -14,40 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t xml:space="preserve">MyBank
-Payee's bank
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5
 </t>
   </si>
   <si>
-    <t>BIK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BIC
-2222
+    <t xml:space="preserve">2
 </t>
   </si>
   <si>
-    <t>Account№</t>
-  </si>
-  <si>
-    <t>INN 123</t>
-  </si>
-  <si>
-    <t>KPP 123456</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account
-№
+    <t>3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2123123
-</t>
-  </si>
-  <si>
-    <t>MycompanyRecipient</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -100,10 +93,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,61 +391,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A4:B4"/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="C5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>